<commit_message>
Review all isr_handler_* functions: add asserts where needed, ensure guidelines are followed.
</commit_message>
<xml_diff>
--- a/ISR-catalog.xlsx
+++ b/ISR-catalog.xlsx
@@ -10,6 +10,9 @@
   <sheets>
     <sheet name="Feuil1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Feuil1!$A$1:$F$45</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="95">
   <si>
     <t xml:space="preserve">File</t>
   </si>
@@ -49,6 +52,9 @@
     <t xml:space="preserve">HandlerHolder</t>
   </si>
   <si>
+    <t xml:space="preserve">NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">REGISTER_EEPROM_ISR_METHOD</t>
   </si>
   <si>
@@ -67,6 +73,9 @@
     <t xml:space="preserve">isr_handler_int_method</t>
   </si>
   <si>
+    <t xml:space="preserve">OK</t>
+  </si>
+  <si>
     <t xml:space="preserve">REGISTER_INT_ISR_FUNCTION</t>
   </si>
   <si>
@@ -79,163 +88,163 @@
     <t xml:space="preserve">NONE</t>
   </si>
   <si>
-    <t xml:space="preserve">interrupts.h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGISTER_ISR_METHOD</t>
+    <t xml:space="preserve">pci.h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REGISTER_PCI_ISR_METHOD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isr_handler_pci_method</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REGISTER_PCI_ISR_FUNCTION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isr_handler_pci_function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REGISTER_PCI_ISR_EMPTY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isr_handler_check_pci_pins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TODO check generated asm code is really optimized!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pulse_timer.h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REGISTER_PULSE_TIMER8_AB_ISR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isr_handler_pulse_timer_overflow, isr_handler_pulse_timer_compare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REGISTER_PULSE_TIMER8_A_ISR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REGISTER_PULSE_TIMER8_B_ISR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">realtime_timer.h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REGISTER_RTT_ISR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isr_handler_rtt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REGISTER_RTT_ISR_METHOD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isr_handler_rtt_method</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REGISTER_RTT_ISR_FUNCTION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isr_handler_rtt_function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REGISTER_RTT_EVENT_ISR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isr_handler_rtt_event</t>
+  </si>
+  <si>
+    <t xml:space="preserve">soft_uart.h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REGISTER_UART_PCI_ISR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isr_handler_check_pci_pins, HandlerHolder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REGISTER_UART_INT_ISR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">timer.h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REGISTER_TIMER_COMPARE_ISR_METHOD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CallbackHandler, isr_handler_check_timer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REGISTER_TIMER_COMPARE_ISR_FUNCTION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REGISTER_TIMER_COMPARE_ISR_EMPTY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No assert at all</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REGISTER_TIMER_OVERFLOW_ISR_METHOD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REGISTER_TIMER_OVERFLOW_ISR_FUNCTION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REGISTER_TIMER_OVERFLOW_ISR_EMPTY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REGISTER_TIMER_CAPTURE_ISR_METHOD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isr_handler_timer_capture_method</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REGISTER_TIMER_CAPTURE_ISR_FUNCTION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isr_handler_timer_capture_function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REGISTER_TIMER_CAPTURE_ISR_EMPTY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uart.h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REGISTER_UATX_ISR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isr_handler_uatx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REGISTER_UARX_ISR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isr_handler_uarx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REGISTER_UART_ISR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isr_handler_uart_tx, isr_handler_uart_rx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">watchdog.h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REGISTER_WATCHDOG_CLOCK_ISR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REGISTER_WATCHDOG_RTT_ISR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REGISTER_WATCHDOG_ISR_METHOD</t>
   </si>
   <si>
     <t xml:space="preserve">CallbackHandler</t>
-  </si>
-  <si>
-    <t xml:space="preserve">For general usage by programs. Maybe useless?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGISTER_ISR_METHOD_RETURN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGISTER_ISR_FUNCTION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Direct call</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pci.h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGISTER_PCI_ISR_METHOD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">isr_handler_pci_method</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGISTER_PCI_ISR_FUNCTION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">isr_handler_pci_function</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGISTER_PCI_ISR_EMPTY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">isr_handler_check_pci_pins</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pulse_timer.h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGISTER_PULSE_TIMER8_AB_ISR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">isr_handler_pulse_timer_overflow, isr_handler_pulse_timer_compare</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGISTER_PULSE_TIMER8_A_ISR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGISTER_PULSE_TIMER8_B_ISR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">realtime_timer.h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGISTER_RTT_ISR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">isr_handler_rtt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGISTER_RTT_ISR_METHOD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">isr_handler_rtt_method</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGISTER_RTT_ISR_FUNCTION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">isr_handler_rtt_function</t>
-  </si>
-  <si>
-    <t xml:space="preserve">soft_uart.h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGISTER_UART_PCI_ISR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">isr_handler_check_pci_pins, HandlerHolder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGISTER_UART_INT_ISR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">timer.h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGISTER_TIMER_COMPARE_ISR_METHOD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGISTER_TIMER_COMPARE_ISR_FUNCTION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGISTER_TIMER_COMPARE_ISR_EMPTY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGISTER_TIMER_OVERFLOW_ISR_METHOD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGISTER_TIMER_OVERFLOW_ISR_FUNCTION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGISTER_TIMER_OVERFLOW_ISR_EMPTY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGISTER_TIMER_CAPTURE_ISR_METHOD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">isr_handler_timer_capture_method</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGISTER_TIMER_CAPTURE_ISR_FUNCTION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">isr_handler_timer_capture_function</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGISTER_TIMER_CAPTURE_ISR_EMPTY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">uart.h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGISTER_UATX_ISR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">isr_handler_uatx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGISTER_UARX_ISR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">isr_handler_uarx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGISTER_UART_ISR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">isr_handler_uart_tx, isr_handler_uart_rx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">watchdog.h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGISTER_WATCHDOG_CLOCK_ISR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGISTER_WATCHDOG_RTT_ISR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGISTER_WATCHDOG_ISR_METHOD</t>
   </si>
   <si>
     <t xml:space="preserve">REGISTER_WATCHDOG_ISR_FUNCTION</t>
@@ -431,17 +440,21 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ48"/>
+  <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -451,9 +464,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="59.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="8.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="7.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="58.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="7" style="4" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="58.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="7" style="4" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="9.13"/>
   </cols>
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -487,407 +500,527 @@
       <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="D2" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>8</v>
+      <c r="D4" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>32</v>
+      <c r="D13" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>35</v>
+        <v>40</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="B17" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="B18" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="B22" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>25</v>
+        <v>49</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>18</v>
+        <v>49</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>25</v>
+        <v>58</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>18</v>
+        <v>60</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="1" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>57</v>
+        <v>20</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="B29" s="1" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>59</v>
+        <v>64</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="1" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>18</v>
+        <v>66</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="B31" s="1" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>63</v>
+        <v>68</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="B32" s="1" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>65</v>
+        <v>8</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="1" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>67</v>
+        <v>8</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="B34" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>8</v>
+        <v>73</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="1" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>8</v>
+        <v>73</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="1" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="1" t="s">
-        <v>72</v>
+      <c r="A37" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>25</v>
+        <v>78</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="1" t="s">
-        <v>73</v>
+      <c r="B38" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>18</v>
+        <v>80</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>75</v>
+      <c r="B40" s="1" t="s">
+        <v>83</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>76</v>
+        <v>84</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="2" t="s">
-        <v>77</v>
+      <c r="B41" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>78</v>
+        <v>86</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="1" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>80</v>
+        <v>88</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="1" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>82</v>
+        <v>90</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="1" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>84</v>
+        <v>92</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="1" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
+        <v>94</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <autoFilter ref="A1:F45"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -895,5 +1028,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add more checks of REGISTER_ macros in AssertChecks to cover more macros.
</commit_message>
<xml_diff>
--- a/ISR-catalog.xlsx
+++ b/ISR-catalog.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="95">
   <si>
     <t xml:space="preserve">File</t>
   </si>
@@ -109,9 +109,6 @@
     <t xml:space="preserve">isr_handler_check_pci_pins</t>
   </si>
   <si>
-    <t xml:space="preserve">TODO check generated asm code is really optimized!</t>
-  </si>
-  <si>
     <t xml:space="preserve">pulse_timer.h</t>
   </si>
   <si>
@@ -200,6 +197,9 @@
   </si>
   <si>
     <t xml:space="preserve">isr_handler_timer_capture_method</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Missing assert on ICP support for existing Timer</t>
   </si>
   <si>
     <t xml:space="preserve">REGISTER_TIMER_CAPTURE_ISR_FUNCTION</t>
@@ -446,7 +446,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
+  <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
@@ -454,7 +454,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
+      <selection pane="bottomLeft" activeCell="F27" activeCellId="0" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -490,7 +490,7 @@
       </c>
       <c r="AMJ1" s="0"/>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -504,7 +504,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
@@ -515,7 +515,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
         <v>12</v>
       </c>
@@ -526,7 +526,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -540,7 +540,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1" t="s">
         <v>17</v>
       </c>
@@ -551,7 +551,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1" t="s">
         <v>19</v>
       </c>
@@ -562,7 +562,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
@@ -576,7 +576,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1" t="s">
         <v>24</v>
       </c>
@@ -587,7 +587,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="1" t="s">
         <v>26</v>
       </c>
@@ -597,138 +597,135 @@
       <c r="D10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="1" t="s">
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="1" t="s">
+      <c r="C16" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="D17" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="C20" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="D20" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="C21" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>16</v>
@@ -736,35 +733,35 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D22" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F22" s="1" t="s">
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="1" t="s">
+      <c r="C23" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="C24" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>16</v>
@@ -772,27 +769,30 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="D26" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -803,7 +803,10 @@
         <v>60</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>16</v>
+        <v>51</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -814,13 +817,13 @@
         <v>20</v>
       </c>
       <c r="D28" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F28" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
         <v>62</v>
       </c>
@@ -834,7 +837,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="1" t="s">
         <v>65</v>
       </c>
@@ -845,7 +848,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="1" t="s">
         <v>67</v>
       </c>
@@ -856,7 +859,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
         <v>69</v>
       </c>
@@ -870,7 +873,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="1" t="s">
         <v>71</v>
       </c>
@@ -881,7 +884,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="1" t="s">
         <v>72</v>
       </c>
@@ -892,7 +895,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="1" t="s">
         <v>74</v>
       </c>
@@ -903,7 +906,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="1" t="s">
         <v>75</v>
       </c>
@@ -914,7 +917,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
         <v>76</v>
       </c>
@@ -928,7 +931,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="2" t="s">
         <v>79</v>
       </c>
@@ -939,7 +942,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="1" t="s">
         <v>81</v>
       </c>
@@ -950,7 +953,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="1" t="s">
         <v>83</v>
       </c>
@@ -961,7 +964,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="1" t="s">
         <v>85</v>
       </c>
@@ -972,7 +975,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="1" t="s">
         <v>87</v>
       </c>
@@ -983,7 +986,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="1" t="s">
         <v>89</v>
       </c>
@@ -994,7 +997,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="1" t="s">
         <v>91</v>
       </c>
@@ -1005,7 +1008,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="1" t="s">
         <v>93</v>
       </c>
@@ -1020,7 +1023,13 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A1:F45"/>
+  <autoFilter ref="A1:F45">
+    <filterColumn colId="3">
+      <customFilters and="true">
+        <customFilter operator="equal" val="KO"/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Fix and refactor a few ISR handlers and REGISTER_ macros. Include sonar macros in AssertChecks.
</commit_message>
<xml_diff>
--- a/ISR-catalog.xlsx
+++ b/ISR-catalog.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="92">
   <si>
     <t xml:space="preserve">File</t>
   </si>
@@ -178,12 +178,6 @@
     <t xml:space="preserve">REGISTER_TIMER_COMPARE_ISR_EMPTY</t>
   </si>
   <si>
-    <t xml:space="preserve">KO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No assert at all</t>
-  </si>
-  <si>
     <t xml:space="preserve">REGISTER_TIMER_OVERFLOW_ISR_METHOD</t>
   </si>
   <si>
@@ -197,9 +191,6 @@
   </si>
   <si>
     <t xml:space="preserve">isr_handler_timer_capture_method</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Missing assert on ICP support for existing Timer</t>
   </si>
   <si>
     <t xml:space="preserve">REGISTER_TIMER_CAPTURE_ISR_FUNCTION</t>
@@ -446,7 +437,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="true">
+  <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
@@ -454,7 +445,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F27" activeCellId="0" sqref="F27"/>
+      <selection pane="bottomLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -490,7 +481,7 @@
       </c>
       <c r="AMJ1" s="0"/>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -503,8 +494,11 @@
       <c r="D2" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E2" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
@@ -514,8 +508,11 @@
       <c r="D3" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E3" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
         <v>12</v>
       </c>
@@ -525,8 +522,11 @@
       <c r="D4" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E4" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -539,8 +539,11 @@
       <c r="D5" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E5" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1" t="s">
         <v>17</v>
       </c>
@@ -550,8 +553,11 @@
       <c r="D6" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E6" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1" t="s">
         <v>19</v>
       </c>
@@ -561,8 +567,11 @@
       <c r="D7" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E7" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
@@ -575,8 +584,11 @@
       <c r="D8" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E8" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1" t="s">
         <v>24</v>
       </c>
@@ -586,8 +598,11 @@
       <c r="D9" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E9" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="1" t="s">
         <v>26</v>
       </c>
@@ -597,8 +612,11 @@
       <c r="D10" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E10" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
@@ -611,8 +629,11 @@
       <c r="D11" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E11" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="1" t="s">
         <v>31</v>
       </c>
@@ -622,8 +643,11 @@
       <c r="D12" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E12" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="1" t="s">
         <v>32</v>
       </c>
@@ -633,8 +657,11 @@
       <c r="D13" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E13" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>33</v>
       </c>
@@ -647,8 +674,11 @@
       <c r="D14" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E14" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="1" t="s">
         <v>36</v>
       </c>
@@ -658,8 +688,11 @@
       <c r="D15" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E15" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="1" t="s">
         <v>38</v>
       </c>
@@ -669,8 +702,11 @@
       <c r="D16" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E16" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="1" t="s">
         <v>40</v>
       </c>
@@ -680,8 +716,11 @@
       <c r="D17" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E17" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>42</v>
       </c>
@@ -694,8 +733,11 @@
       <c r="D18" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E18" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="1" t="s">
         <v>45</v>
       </c>
@@ -705,8 +747,11 @@
       <c r="D19" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E19" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
         <v>46</v>
       </c>
@@ -719,8 +764,11 @@
       <c r="D20" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E20" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="1" t="s">
         <v>49</v>
       </c>
@@ -728,6 +776,9 @@
         <v>48</v>
       </c>
       <c r="D21" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="3" t="s">
         <v>16</v>
       </c>
     </row>
@@ -739,15 +790,15 @@
         <v>20</v>
       </c>
       <c r="D22" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>48</v>
@@ -755,10 +806,13 @@
       <c r="D23" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E23" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>48</v>
@@ -766,105 +820,117 @@
       <c r="D24" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="E24" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>52</v>
+        <v>16</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>58</v>
+        <v>16</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>58</v>
+        <v>16</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>16</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="C30" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="D30" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D29" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="1" t="s">
+      <c r="C31" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="D31" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D30" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="1" t="s">
+      <c r="B32" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>8</v>
@@ -872,10 +938,13 @@
       <c r="D32" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E32" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>8</v>
@@ -883,32 +952,41 @@
       <c r="D33" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E33" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>20</v>
@@ -916,106 +994,136 @@
       <c r="D36" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E36" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="C38" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="D38" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D37" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="2" t="s">
+      <c r="C39" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="D39" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D38" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="1" t="s">
+      <c r="C40" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="D40" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D39" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="1" t="s">
+      <c r="C41" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="D41" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D40" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="1" t="s">
+      <c r="C42" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="D42" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D41" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="1" t="s">
+      <c r="C43" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="D43" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D42" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="1" t="s">
+      <c r="C44" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="D44" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D43" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="1" t="s">
+      <c r="C45" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C44" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>94</v>
-      </c>
       <c r="D45" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E45" s="3" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1023,13 +1131,7 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A1:F45">
-    <filterColumn colId="3">
-      <customFilters and="true">
-        <customFilter operator="equal" val="KO"/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:F45"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Update list of REGISTER_ macros (new sonar macros).
</commit_message>
<xml_diff>
--- a/ISR-catalog.xlsx
+++ b/ISR-catalog.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Feuil1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Feuil1!$A$1:$F$45</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Feuil1!$A$1:$F$48</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="101">
   <si>
     <t xml:space="preserve">File</t>
   </si>
@@ -289,6 +289,18 @@
     <t xml:space="preserve">isr_handler_sonar_pci_function</t>
   </si>
   <si>
+    <t xml:space="preserve">REGISTER_HCSR04_RTT_TIMEOUT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isr_handler::sonar_rtt_change</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REGISTER_HCSR04_RTT_TIMEOUT_METHOD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REGISTER_HCSR04_RTT_TIMEOUT_FUNCTION</t>
+  </si>
+  <si>
     <t xml:space="preserve">REGISTER_MULTI_HCSR04_PCI_ISR_METHOD</t>
   </si>
   <si>
@@ -299,6 +311,21 @@
   </si>
   <si>
     <t xml:space="preserve">isr_handler_multi_sonar_pci_function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REGISTER_MULTI_HCSR04_RTT_TIMEOUT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isr_handler::multi_sonar_rtt_change</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REGISTER_MULTI_HCSR04_RTT_TIMEOUT_METHOD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isr_handler::multi_sonar_rtt_change, CallbackHandler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REGISTER_MULTI_HCSR04_RTT_TIMEOUT_FUNCTION</t>
   </si>
 </sst>
 </file>
@@ -382,7 +409,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -419,6 +446,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -440,18 +471,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ1048576"/>
+  <dimension ref="A1:AMJ51"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+      <selection pane="bottomLeft" activeCell="C48" activeCellId="0" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="40.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="48.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="59.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="8.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="7.57"/>
@@ -1100,38 +1131,83 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="1" t="s">
+      <c r="B44" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C44" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="D44" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="1" t="s">
+      <c r="B45" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C45" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="D45" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="C46" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>99</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F45"/>
+  <autoFilter ref="A1:F48"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>